<commit_message>
fixed some PR stuff+results
</commit_message>
<xml_diff>
--- a/HS.BA.Unemployment.Employment.byState.xlsx
+++ b/HS.BA.Unemployment.Employment.byState.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t xml:space="preserve">WY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR</t>
   </si>
   <si>
     <t xml:space="preserve">Deaf</t>
@@ -558,19 +561,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>82.4</v>
+        <v>82.1</v>
       </c>
       <c r="C2" t="n">
         <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>88.7</v>
+        <v>88.6</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-6.3</v>
+        <v>-6.5</v>
       </c>
       <c r="G2" t="n">
         <v>0.1</v>
@@ -1747,6 +1750,29 @@
       </c>
       <c r="G53" t="n">
         <v>1.6</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>65.3</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D54" t="n">
+        <v>82.8</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-17.5</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.1</v>
       </c>
     </row>
   </sheetData>
@@ -2982,6 +3008,29 @@
         <v>1.9</v>
       </c>
     </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>16.2</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D54" t="n">
+        <v>28.8</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-12.6</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -3030,7 +3079,7 @@
         <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -4213,6 +4262,29 @@
       </c>
       <c r="G53" t="n">
         <v>1.8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="D54" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-2.9</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -4257,19 +4329,19 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>51.2</v>
+        <v>50.9</v>
       </c>
       <c r="C2" t="n">
         <v>0.1</v>
       </c>
       <c r="D2" t="n">
-        <v>74.1</v>
+        <v>73.9</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>-22.9</v>
+        <v>-23</v>
       </c>
       <c r="G2" t="n">
         <v>0.1</v>
@@ -5446,6 +5518,29 @@
       </c>
       <c r="G53" t="n">
         <v>2.9</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>28.1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D54" t="n">
+        <v>52.6</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="F54" t="n">
+        <v>-24.5</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>
@@ -5467,10 +5562,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
@@ -5478,10 +5573,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>19578200</v>
+        <v>19806100</v>
       </c>
       <c r="C2" t="n">
-        <v>775948400</v>
+        <v>783376800</v>
       </c>
     </row>
     <row r="3">
@@ -6043,6 +6138,17 @@
       </c>
       <c r="C53" t="n">
         <v>1418100</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>59</v>
+      </c>
+      <c r="B54" t="n">
+        <v>227900</v>
+      </c>
+      <c r="C54" t="n">
+        <v>7428400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>